<commit_message>
Additional comments were added.
</commit_message>
<xml_diff>
--- a/src/main/resources/water_analysis_format.xlsx
+++ b/src/main/resources/water_analysis_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Eviatar\IdeaProjects\Final-Project-Maven\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1A5DF7-1658-4CD5-89CB-5268B7EBE1E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39077B0-698F-4A7A-9508-71F14690B1E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -543,7 +543,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +574,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="5">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>34</v>
@@ -909,6 +909,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E7F5E094DC5E2948848481730747906E" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e2ee9f7bc6b98ccdfe56e2ead30eeb8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="766aba29-3875-45b2-af99-ed533f892980" xmlns:ns3="aa781d43-3968-4c36-8c04-92512332ecb8" xmlns:ns4="5144a9a3-a2b0-4147-97d3-94d65b917612" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4729878b84af48a8c52b489a8c554d66" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1127,41 +1145,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC88DF9A-5CBD-4A06-A933-7CDFE52F4587}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C030DB9-7096-45FC-9C50-E61F30C238BB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="766aba29-3875-45b2-af99-ed533f892980"/>
-    <ds:schemaRef ds:uri="aa781d43-3968-4c36-8c04-92512332ecb8"/>
-    <ds:schemaRef ds:uri="5144a9a3-a2b0-4147-97d3-94d65b917612"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1186,9 +1173,22 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C030DB9-7096-45FC-9C50-E61F30C238BB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC88DF9A-5CBD-4A06-A933-7CDFE52F4587}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="766aba29-3875-45b2-af99-ed533f892980"/>
+    <ds:schemaRef ds:uri="aa781d43-3968-4c36-8c04-92512332ecb8"/>
+    <ds:schemaRef ds:uri="5144a9a3-a2b0-4147-97d3-94d65b917612"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>